<commit_message>
Preparing repository for submission
</commit_message>
<xml_diff>
--- a/input_files/CST_storage_case_charging.xlsx
+++ b/input_files/CST_storage_case_charging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awongel/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944D1AB0-228F-CE4A-9111-FC72CFBBCDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC84E8F6-C9F3-7E4D-86DF-E97449C739B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -299,15 +299,6 @@
     <t>molten-salt-store glasspoint</t>
   </si>
   <si>
-    <t>heat_storage</t>
-  </si>
-  <si>
-    <t>heat storage link in</t>
-  </si>
-  <si>
-    <t>heat storage link out</t>
-  </si>
-  <si>
     <t>csp direct link</t>
   </si>
   <si>
@@ -320,13 +311,13 @@
     <t>cst direct</t>
   </si>
   <si>
-    <t>Store</t>
-  </si>
-  <si>
     <t>marginal_cost_storage</t>
   </si>
   <si>
     <t>cst_storage</t>
+  </si>
+  <si>
+    <t>StorageUnit</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1504,7 +1495,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1512,7 +1503,7 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1699,7 +1690,7 @@
         <v>15</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>19</v>
@@ -1740,13 +1731,13 @@
         <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
         <v>77</v>
       </c>
       <c r="D51" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I51" s="15" t="s">
         <v>79</v>
@@ -1771,13 +1762,13 @@
         <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E52" t="s">
         <v>80</v>
@@ -1789,146 +1780,100 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" t="s">
         <v>89</v>
       </c>
-      <c r="C53" t="s">
-        <v>89</v>
-      </c>
-      <c r="D53" t="s">
-        <v>92</v>
-      </c>
-      <c r="E53" t="s">
-        <v>88</v>
-      </c>
-      <c r="I53" s="15"/>
-      <c r="K53" s="16">
-        <v>1E-8</v>
-      </c>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
+      <c r="I53" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="K53" s="16"/>
+      <c r="M53" s="1">
+        <v>-1E-8</v>
+      </c>
+      <c r="N53" t="b">
+        <v>1</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="P53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q53" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D54" t="s">
-        <v>88</v>
-      </c>
-      <c r="E54" t="s">
         <v>80</v>
       </c>
-      <c r="I54" s="15"/>
-      <c r="K54" s="16">
-        <v>1E-8</v>
-      </c>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
+      <c r="I54" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="P54" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55" t="s">
-        <v>87</v>
-      </c>
-      <c r="C55" t="s">
-        <v>83</v>
-      </c>
-      <c r="D55" t="s">
-        <v>88</v>
-      </c>
-      <c r="I55" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="K55" s="16"/>
-      <c r="M55" s="1">
-        <v>-1E-8</v>
-      </c>
-      <c r="N55" t="b">
-        <v>1</v>
-      </c>
-      <c r="O55" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="P55" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q55" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" t="s">
-        <v>81</v>
-      </c>
-      <c r="C56" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" t="s">
-        <v>80</v>
-      </c>
-      <c r="I56" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="O56" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="P56" s="5" t="s">
-        <v>79</v>
-      </c>
+      <c r="A55" s="6"/>
+      <c r="I55" s="15"/>
+      <c r="K55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57" s="6"/>
-      <c r="I57" s="15"/>
-      <c r="K57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>27</v>
-      </c>
+      <c r="A61" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A63" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="7"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
         <v>55</v>
       </c>
-      <c r="L64" s="7"/>
-      <c r="M64" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>